<commit_message>
Excel files with tickers data.
</commit_message>
<xml_diff>
--- a/tickers/backup/tickers_france.xlsx
+++ b/tickers/backup/tickers_france.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://publicisgroupe-my.sharepoint.com/personal/piediot_publicisgroupe_net/Documents/03 - PERSO/Trading/YourStockPortfolio/tickers/backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2A652B5783B7832E4D4B2BFC09F57E113B874D4C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07E3B41C-EF29-489A-8658-BB59632147B5}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_2A652B5783B7832E4D4B2BFC09F57E113B874D4C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF0479C6-9B0E-48CC-8A0D-018AF1FC11B4}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21168" yWindow="-100" windowWidth="18809" windowHeight="11243" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STOXX 600" sheetId="1" r:id="rId1"/>
@@ -688,6 +688,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1034,11 +1035,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -2226,8 +2230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>